<commit_message>
Did way to much fucking matlab code for a lab but screw it
</commit_message>
<xml_diff>
--- a/335Lab/Lab 2/Data/AverageVelocities.xlsx
+++ b/335Lab/Lab 2/Data/AverageVelocities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Class Work\Current\ME335\335 Lab\Lab 2\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Class Work\Current\ME335\335Lab\Lab 2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97DBF00E-2C0C-4FE4-9193-06CA35E6E6DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8C3A5F-CE44-49F3-8440-E864155FA594}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="2160" windowWidth="23040" windowHeight="12216" xr2:uid="{8F385075-BD0B-654F-A0F3-8047B2A0C05C}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{8F385075-BD0B-654F-A0F3-8047B2A0C05C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -447,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E9BAB3-2E29-344B-A900-0A4F9CE6DDD1}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -458,390 +458,357 @@
     <col min="1" max="1" width="7.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>-2.87</v>
       </c>
       <c r="B2">
-        <v>-2.87</v>
+        <v>9.2258999999999993</v>
       </c>
       <c r="C2">
-        <v>9.2258999999999993</v>
+        <v>9.9579000000000004</v>
       </c>
       <c r="D2">
-        <v>9.9579000000000004</v>
+        <v>7.2622900000000001</v>
       </c>
       <c r="E2">
-        <v>7.2622900000000001</v>
+        <v>7.7402300000000004</v>
       </c>
       <c r="F2">
-        <v>7.7402300000000004</v>
+        <v>5.4980500000000001</v>
       </c>
       <c r="G2">
-        <v>5.4980500000000001</v>
+        <v>5.5517200000000004</v>
       </c>
       <c r="H2">
-        <v>5.5517200000000004</v>
+        <v>3.8959800000000002</v>
       </c>
       <c r="I2">
-        <v>3.8959800000000002</v>
-      </c>
-      <c r="J2">
         <v>3.5211700000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>-2.54</v>
       </c>
       <c r="B3">
-        <v>-2.54</v>
+        <v>11.6814</v>
       </c>
       <c r="C3">
-        <v>11.6814</v>
+        <v>11.8642</v>
       </c>
       <c r="D3">
-        <v>11.8642</v>
+        <v>9.1379199999999994</v>
       </c>
       <c r="E3">
-        <v>9.1379199999999994</v>
+        <v>10.716200000000001</v>
       </c>
       <c r="F3">
-        <v>10.716200000000001</v>
+        <v>6.6918899999999999</v>
       </c>
       <c r="G3">
-        <v>6.6918899999999999</v>
+        <v>6.9829800000000004</v>
       </c>
       <c r="H3">
-        <v>6.9829800000000004</v>
+        <v>4.6583899999999998</v>
       </c>
       <c r="I3">
-        <v>4.6583899999999998</v>
-      </c>
-      <c r="J3">
         <v>4.4594300000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>-2.14</v>
       </c>
       <c r="B4">
-        <v>2.14</v>
+        <v>12.8774</v>
       </c>
       <c r="C4">
-        <v>12.8774</v>
+        <v>13.4964</v>
       </c>
       <c r="D4">
-        <v>13.4964</v>
+        <v>10.264699999999999</v>
       </c>
       <c r="E4">
-        <v>10.264699999999999</v>
+        <v>11.3866</v>
       </c>
       <c r="F4">
-        <v>11.3866</v>
+        <v>7.7682450000000003</v>
       </c>
       <c r="G4">
-        <v>7.7682450000000003</v>
+        <v>7.9386400000000004</v>
       </c>
       <c r="H4">
-        <v>7.9386400000000004</v>
+        <v>5.2721910000000003</v>
       </c>
       <c r="I4">
-        <v>5.2721910000000003</v>
-      </c>
-      <c r="J4">
         <v>5.1642099999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>-1.66</v>
       </c>
       <c r="B5">
-        <v>-1.66</v>
+        <v>13.4688</v>
       </c>
       <c r="C5">
-        <v>13.4688</v>
+        <v>14.410500000000001</v>
       </c>
       <c r="D5">
-        <v>14.410500000000001</v>
+        <v>10.730700000000001</v>
       </c>
       <c r="E5">
-        <v>10.730700000000001</v>
+        <v>11.4634</v>
       </c>
       <c r="F5">
-        <v>11.4634</v>
+        <v>8.3095400000000001</v>
       </c>
       <c r="G5">
-        <v>8.3095400000000001</v>
+        <v>8.3910499999999999</v>
       </c>
       <c r="H5">
-        <v>8.3910499999999999</v>
+        <v>5.7173800000000004</v>
       </c>
       <c r="I5">
-        <v>5.7173800000000004</v>
-      </c>
-      <c r="J5">
         <v>5.6326599999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>-0.96</v>
       </c>
       <c r="B6">
-        <v>-0.96</v>
+        <v>13.5783</v>
       </c>
       <c r="C6">
-        <v>13.5783</v>
+        <v>14.450900000000001</v>
       </c>
       <c r="D6">
-        <v>14.450900000000001</v>
+        <v>10.695600000000001</v>
       </c>
       <c r="E6">
-        <v>10.695600000000001</v>
+        <v>11.1469</v>
       </c>
       <c r="F6">
-        <v>11.1469</v>
+        <v>8.2248699999999992</v>
       </c>
       <c r="G6">
-        <v>8.2248699999999992</v>
+        <v>8.5873699999999999</v>
       </c>
       <c r="H6">
-        <v>8.5873699999999999</v>
+        <v>5.6718000000000002</v>
       </c>
       <c r="I6">
-        <v>5.6718000000000002</v>
-      </c>
-      <c r="J6">
         <v>5.6879900000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>0</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>13.5022</v>
       </c>
       <c r="C7">
-        <v>13.5022</v>
+        <v>14.1783</v>
       </c>
       <c r="D7">
-        <v>14.1783</v>
+        <v>10.712400000000001</v>
       </c>
       <c r="E7">
-        <v>10.712400000000001</v>
+        <v>11.2971</v>
       </c>
       <c r="F7">
-        <v>11.2971</v>
+        <v>8.81128</v>
       </c>
       <c r="G7">
-        <v>8.81128</v>
+        <v>8.4280709999999992</v>
       </c>
       <c r="H7">
-        <v>8.4280709999999992</v>
+        <v>5.6463299999999998</v>
       </c>
       <c r="I7">
-        <v>5.6463299999999998</v>
-      </c>
-      <c r="J7">
         <v>5.5425899999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>0.96</v>
       </c>
       <c r="B8">
-        <v>0.96</v>
+        <v>12.8399</v>
       </c>
       <c r="C8">
-        <v>12.8399</v>
+        <v>14.2308</v>
       </c>
       <c r="D8">
-        <v>14.2308</v>
+        <v>10.167199999999999</v>
       </c>
       <c r="E8">
-        <v>10.167199999999999</v>
+        <v>10.695499999999999</v>
       </c>
       <c r="F8">
-        <v>10.695499999999999</v>
+        <v>7.8680599999999998</v>
       </c>
       <c r="G8">
-        <v>7.8680599999999998</v>
+        <v>8.4300660000000001</v>
       </c>
       <c r="H8">
-        <v>8.4300660000000001</v>
+        <v>5.4496000000000002</v>
       </c>
       <c r="I8">
-        <v>5.4496000000000002</v>
-      </c>
-      <c r="J8">
         <v>5.5757399999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1.66</v>
       </c>
       <c r="B9">
-        <v>1.66</v>
+        <v>12.0571</v>
       </c>
       <c r="C9">
-        <v>12.0571</v>
+        <v>14.7097</v>
       </c>
       <c r="D9">
-        <v>14.7097</v>
+        <v>9.6627200000000002</v>
       </c>
       <c r="E9">
-        <v>9.6627200000000002</v>
+        <v>9.9958899999999993</v>
       </c>
       <c r="F9">
-        <v>9.9958899999999993</v>
+        <v>7.3948099999999997</v>
       </c>
       <c r="G9">
-        <v>7.3948099999999997</v>
+        <v>7.9641999999999999</v>
       </c>
       <c r="H9">
-        <v>7.9641999999999999</v>
+        <v>5.1971299999999996</v>
       </c>
       <c r="I9">
-        <v>5.1971299999999996</v>
-      </c>
-      <c r="J9">
         <v>5.30213</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2.14</v>
       </c>
       <c r="B10">
-        <v>2.14</v>
+        <v>11.6225</v>
       </c>
       <c r="C10">
-        <v>11.6225</v>
+        <v>12.6617</v>
       </c>
       <c r="D10">
-        <v>12.6617</v>
+        <v>9.1468699999999998</v>
       </c>
       <c r="E10">
-        <v>9.1468699999999998</v>
+        <v>10.0749</v>
       </c>
       <c r="F10">
-        <v>10.0749</v>
+        <v>7.0183099999999996</v>
       </c>
       <c r="G10">
-        <v>7.0183099999999996</v>
+        <v>7.3258999999999999</v>
       </c>
       <c r="H10">
-        <v>7.3258999999999999</v>
+        <v>4.9429499999999997</v>
       </c>
       <c r="I10">
-        <v>4.9429499999999997</v>
-      </c>
-      <c r="J10">
         <v>4.7884700000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>2.54</v>
       </c>
       <c r="B11">
-        <v>2.54</v>
+        <v>10.845000000000001</v>
       </c>
       <c r="C11">
-        <v>10.845000000000001</v>
+        <v>11.5113</v>
       </c>
       <c r="D11">
-        <v>11.5113</v>
+        <v>8.6439599999999999</v>
       </c>
       <c r="E11">
-        <v>8.6439599999999999</v>
+        <v>9.0748999999999995</v>
       </c>
       <c r="F11">
-        <v>9.0748999999999995</v>
+        <v>6.5254700000000003</v>
       </c>
       <c r="G11">
-        <v>6.5254700000000003</v>
+        <v>6.6096500000000002</v>
       </c>
       <c r="H11">
-        <v>6.6096500000000002</v>
+        <v>4.4989499999999998</v>
       </c>
       <c r="I11">
-        <v>4.4989499999999998</v>
-      </c>
-      <c r="J11">
         <v>4.3094799999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>2.87</v>
       </c>
       <c r="B12">
-        <v>2.87</v>
+        <v>9.2630800000000004</v>
       </c>
       <c r="C12">
-        <v>9.2630800000000004</v>
+        <v>9.7662800000000001</v>
       </c>
       <c r="D12">
-        <v>9.7662800000000001</v>
+        <v>7.4408000000000003</v>
       </c>
       <c r="E12">
-        <v>7.4408000000000003</v>
+        <v>7.4586199999999998</v>
       </c>
       <c r="F12">
-        <v>7.4586199999999998</v>
+        <v>5.6287200000000004</v>
       </c>
       <c r="G12">
-        <v>5.6287200000000004</v>
+        <v>5.4375999999999998</v>
       </c>
       <c r="H12">
-        <v>5.4375999999999998</v>
+        <v>3.8572600000000001</v>
       </c>
       <c r="I12">
-        <v>3.8572600000000001</v>
-      </c>
-      <c r="J12">
         <v>3.3584000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -849,11 +816,10 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -862,21 +828,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C35235A0CBEA4E4BA44A492B72CB0F55" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70e5c958f602f45486ea9c9e3e1161eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6112e395-b193-4778-b513-460523810ab5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="df585931453734ed62ad13ba882f2bc2" ns2:_="">
     <xsd:import namespace="6112e395-b193-4778-b513-460523810ab5"/>
@@ -1008,24 +959,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69A6E76E-B456-4173-B04E-AAD867A954CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{752821D1-C181-4644-ABF0-CDCC8C499165}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{530C1D90-556C-4950-90F5-1F2F84D012E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1041,4 +990,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{752821D1-C181-4644-ABF0-CDCC8C499165}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69A6E76E-B456-4173-B04E-AAD867A954CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>